<commit_message>
Added metadata files and fixed f0_voicing_dur typos
</commit_message>
<xml_diff>
--- a/klatt_synthesis/experimental_stimuli/f0_voicing_dur/klatt_params.xlsx
+++ b/klatt_synthesis/experimental_stimuli/f0_voicing_dur/klatt_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughe\Documents\CNN_Perceptual_Integration_Channel_Bias\Experiment\klatt_synthesis\experimental_stimuli\f0_voicing_dur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4BF267-A239-416B-BEA0-903360674568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142E65F5-6245-4D87-8F01-786B8AA9516D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6078420B-0BAE-46C7-A6CE-83D12546AFEA}"/>
   </bookViews>
@@ -37,12 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>HighF1_LongVoicing</t>
-  </si>
-  <si>
-    <t>HighF1_ShortVoicing</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -106,10 +100,16 @@
     <t>ClosureVoicingDur</t>
   </si>
   <si>
-    <t>LowF1_LongVoicing</t>
-  </si>
-  <si>
-    <t>LowF1_ShortVoicing</t>
+    <t>Highf0_LongVoicing</t>
+  </si>
+  <si>
+    <t>Highf0_ShortVoicing</t>
+  </si>
+  <si>
+    <t>Lowf0_LongVoicing</t>
+  </si>
+  <si>
+    <t>Lowf0_ShortVoicing</t>
   </si>
 </sst>
 </file>
@@ -471,79 +471,79 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0.20499999999999999</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>0.20499999999999999</v>

</xml_diff>